<commit_message>
sprint 2 notebook opgekuist
</commit_message>
<xml_diff>
--- a/data/Inside Airbnb Data Dictionary.xlsx
+++ b/data/Inside Airbnb Data Dictionary.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24430"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24527"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\bavop\Documents\Bavo\UGent\UGent 2021-2022\Machinaal Leren\Project\ProjectML\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D28075F4-D247-4793-83DC-E72362461FDB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D8B90FE3-73AF-425F-BD69-B890F56AA010}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="listings.csv detail v4" sheetId="1" r:id="rId1"/>
@@ -723,9 +723,6 @@
   </cellStyleXfs>
   <cellXfs count="16">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
@@ -757,6 +754,9 @@
     <xf numFmtId="0" fontId="7" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="2" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -1144,1336 +1144,1336 @@
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
       <pane ySplit="8" topLeftCell="A9" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="A11" sqref="A11"/>
+      <selection pane="bottomLeft" activeCell="A76" sqref="A76"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="13.2" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="25.109375" customWidth="1"/>
-    <col min="2" max="3" width="14.44140625" customWidth="1"/>
-    <col min="4" max="5" width="43.6640625" customWidth="1"/>
-    <col min="6" max="1025" width="14.44140625" customWidth="1"/>
+    <col min="1" max="1" width="25.140625" customWidth="1"/>
+    <col min="2" max="3" width="14.42578125" customWidth="1"/>
+    <col min="4" max="5" width="43.7109375" customWidth="1"/>
+    <col min="6" max="1025" width="14.42578125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" ht="17.399999999999999" x14ac:dyDescent="0.3">
-      <c r="A1" s="2" t="s">
+    <row r="1" spans="1:5" ht="18" x14ac:dyDescent="0.25">
+      <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="3"/>
-    </row>
-    <row r="2" spans="1:5" ht="13.8" x14ac:dyDescent="0.25">
-      <c r="A2" s="4"/>
-      <c r="B2" s="3"/>
-    </row>
-    <row r="3" spans="1:5" ht="13.8" x14ac:dyDescent="0.25">
-      <c r="A3" s="4" t="s">
+      <c r="B1" s="2"/>
+    </row>
+    <row r="2" spans="1:5" ht="15" x14ac:dyDescent="0.25">
+      <c r="A2" s="3"/>
+      <c r="B2" s="2"/>
+    </row>
+    <row r="3" spans="1:5" ht="15" x14ac:dyDescent="0.25">
+      <c r="A3" s="3" t="s">
         <v>1</v>
       </c>
-      <c r="B3" s="5" t="s">
+      <c r="B3" s="4" t="s">
         <v>2</v>
       </c>
     </row>
-    <row r="4" spans="1:5" ht="13.8" x14ac:dyDescent="0.25">
-      <c r="A4" s="4" t="s">
+    <row r="4" spans="1:5" ht="15" x14ac:dyDescent="0.25">
+      <c r="A4" s="3" t="s">
         <v>3</v>
       </c>
-      <c r="B4" s="5">
+      <c r="B4" s="4">
         <v>4</v>
       </c>
     </row>
-    <row r="5" spans="1:5" ht="13.8" x14ac:dyDescent="0.25">
-      <c r="A5" s="4" t="s">
+    <row r="5" spans="1:5" ht="15" x14ac:dyDescent="0.25">
+      <c r="A5" s="3" t="s">
         <v>4</v>
       </c>
-      <c r="B5" s="6">
+      <c r="B5" s="5">
         <v>44044</v>
       </c>
     </row>
-    <row r="6" spans="1:5" ht="13.8" x14ac:dyDescent="0.25">
-      <c r="A6" s="4" t="s">
+    <row r="6" spans="1:5" ht="15" x14ac:dyDescent="0.25">
+      <c r="A6" s="3" t="s">
         <v>5</v>
       </c>
-      <c r="B6" s="1"/>
-      <c r="C6" s="1"/>
-      <c r="D6" s="1"/>
-      <c r="E6" s="1"/>
-    </row>
-    <row r="7" spans="1:5" ht="13.8" x14ac:dyDescent="0.25">
-      <c r="A7" s="3"/>
-      <c r="B7" s="3"/>
-      <c r="C7" s="3"/>
-      <c r="D7" s="3"/>
-      <c r="E7" s="3"/>
-    </row>
-    <row r="8" spans="1:5" ht="13.8" x14ac:dyDescent="0.25">
-      <c r="A8" s="7" t="s">
+      <c r="B6" s="15"/>
+      <c r="C6" s="15"/>
+      <c r="D6" s="15"/>
+      <c r="E6" s="15"/>
+    </row>
+    <row r="7" spans="1:5" ht="14.25" x14ac:dyDescent="0.2">
+      <c r="A7" s="2"/>
+      <c r="B7" s="2"/>
+      <c r="C7" s="2"/>
+      <c r="D7" s="2"/>
+      <c r="E7" s="2"/>
+    </row>
+    <row r="8" spans="1:5" ht="15" x14ac:dyDescent="0.2">
+      <c r="A8" s="6" t="s">
         <v>6</v>
       </c>
-      <c r="B8" s="7" t="s">
+      <c r="B8" s="6" t="s">
         <v>7</v>
       </c>
-      <c r="C8" s="7" t="s">
+      <c r="C8" s="6" t="s">
         <v>8</v>
       </c>
-      <c r="D8" s="7" t="s">
+      <c r="D8" s="6" t="s">
         <v>5</v>
       </c>
-      <c r="E8" s="7" t="s">
+      <c r="E8" s="6" t="s">
         <v>9</v>
       </c>
     </row>
-    <row r="9" spans="1:5" ht="13.8" x14ac:dyDescent="0.25">
-      <c r="A9" s="8" t="s">
+    <row r="9" spans="1:5" ht="14.25" x14ac:dyDescent="0.2">
+      <c r="A9" s="14" t="s">
         <v>10</v>
       </c>
-      <c r="B9" s="8" t="s">
+      <c r="B9" s="7" t="s">
         <v>11</v>
       </c>
-      <c r="C9" s="8"/>
-      <c r="D9" s="9" t="s">
+      <c r="C9" s="7"/>
+      <c r="D9" s="8" t="s">
         <v>12</v>
       </c>
-      <c r="E9" s="9"/>
-    </row>
-    <row r="10" spans="1:5" ht="13.8" x14ac:dyDescent="0.25">
-      <c r="A10" s="8" t="s">
+      <c r="E9" s="8"/>
+    </row>
+    <row r="10" spans="1:5" ht="14.25" x14ac:dyDescent="0.2">
+      <c r="A10" s="7" t="s">
         <v>13</v>
       </c>
-      <c r="B10" s="8" t="s">
+      <c r="B10" s="7" t="s">
         <v>14</v>
       </c>
-      <c r="C10" s="8" t="s">
+      <c r="C10" s="7" t="s">
         <v>15</v>
       </c>
-      <c r="D10" s="9"/>
-      <c r="E10" s="9"/>
-    </row>
-    <row r="11" spans="1:5" ht="13.8" x14ac:dyDescent="0.25">
-      <c r="A11" s="8" t="s">
+      <c r="D10" s="8"/>
+      <c r="E10" s="8"/>
+    </row>
+    <row r="11" spans="1:5" ht="14.25" x14ac:dyDescent="0.2">
+      <c r="A11" s="7" t="s">
         <v>16</v>
       </c>
-      <c r="B11" s="8" t="s">
+      <c r="B11" s="7" t="s">
         <v>17</v>
       </c>
-      <c r="C11" s="8" t="s">
+      <c r="C11" s="7" t="s">
         <v>15</v>
       </c>
-      <c r="D11" s="9" t="s">
+      <c r="D11" s="8" t="s">
         <v>18</v>
       </c>
-      <c r="E11" s="9"/>
-    </row>
-    <row r="12" spans="1:5" ht="27.6" x14ac:dyDescent="0.25">
-      <c r="A12" s="8" t="s">
+      <c r="E11" s="8"/>
+    </row>
+    <row r="12" spans="1:5" ht="28.5" x14ac:dyDescent="0.2">
+      <c r="A12" s="7" t="s">
         <v>19</v>
       </c>
-      <c r="B12" s="8" t="s">
+      <c r="B12" s="7" t="s">
         <v>20</v>
       </c>
-      <c r="C12" s="8" t="s">
+      <c r="C12" s="7" t="s">
         <v>15</v>
       </c>
-      <c r="D12" s="9" t="s">
+      <c r="D12" s="8" t="s">
         <v>21</v>
       </c>
-      <c r="E12" s="9"/>
-    </row>
-    <row r="13" spans="1:5" ht="13.8" x14ac:dyDescent="0.25">
-      <c r="A13" s="8" t="s">
+      <c r="E12" s="8"/>
+    </row>
+    <row r="13" spans="1:5" ht="14.25" x14ac:dyDescent="0.2">
+      <c r="A13" s="14" t="s">
         <v>22</v>
       </c>
-      <c r="B13" s="8" t="s">
+      <c r="B13" s="7" t="s">
         <v>14</v>
       </c>
-      <c r="C13" s="8"/>
-      <c r="D13" s="9" t="s">
+      <c r="C13" s="7"/>
+      <c r="D13" s="8" t="s">
         <v>23</v>
       </c>
-      <c r="E13" s="9"/>
-    </row>
-    <row r="14" spans="1:5" ht="13.8" x14ac:dyDescent="0.25">
-      <c r="A14" s="8" t="s">
+      <c r="E13" s="8"/>
+    </row>
+    <row r="14" spans="1:5" ht="14.25" x14ac:dyDescent="0.2">
+      <c r="A14" s="14" t="s">
         <v>24</v>
       </c>
-      <c r="B14" s="8" t="s">
+      <c r="B14" s="7" t="s">
         <v>14</v>
       </c>
-      <c r="C14" s="8"/>
-      <c r="D14" s="9" t="s">
+      <c r="C14" s="7"/>
+      <c r="D14" s="8" t="s">
         <v>25</v>
       </c>
-      <c r="E14" s="9"/>
-    </row>
-    <row r="15" spans="1:5" ht="13.8" x14ac:dyDescent="0.25">
-      <c r="A15" s="8" t="s">
+      <c r="E14" s="8"/>
+    </row>
+    <row r="15" spans="1:5" ht="14.25" x14ac:dyDescent="0.2">
+      <c r="A15" s="14" t="s">
         <v>26</v>
       </c>
-      <c r="B15" s="8" t="s">
+      <c r="B15" s="7" t="s">
         <v>14</v>
       </c>
-      <c r="C15" s="8"/>
-      <c r="D15" s="9" t="s">
+      <c r="C15" s="7"/>
+      <c r="D15" s="8" t="s">
         <v>27</v>
       </c>
-      <c r="E15" s="9"/>
-    </row>
-    <row r="16" spans="1:5" ht="27.6" x14ac:dyDescent="0.25">
-      <c r="A16" s="8" t="s">
+      <c r="E15" s="8"/>
+    </row>
+    <row r="16" spans="1:5" ht="28.5" x14ac:dyDescent="0.2">
+      <c r="A16" s="7" t="s">
         <v>28</v>
       </c>
-      <c r="B16" s="8" t="s">
+      <c r="B16" s="7" t="s">
         <v>14</v>
       </c>
-      <c r="C16" s="8"/>
-      <c r="D16" s="9" t="s">
+      <c r="C16" s="7"/>
+      <c r="D16" s="8" t="s">
         <v>29</v>
       </c>
-      <c r="E16" s="9"/>
-    </row>
-    <row r="17" spans="1:5" ht="13.8" x14ac:dyDescent="0.25">
-      <c r="A17" s="8" t="s">
+      <c r="E16" s="8"/>
+    </row>
+    <row r="17" spans="1:5" ht="14.25" x14ac:dyDescent="0.2">
+      <c r="A17" s="7" t="s">
         <v>30</v>
       </c>
-      <c r="B17" s="8" t="s">
+      <c r="B17" s="7" t="s">
         <v>11</v>
       </c>
-      <c r="C17" s="8"/>
-      <c r="D17" s="9" t="s">
+      <c r="C17" s="7"/>
+      <c r="D17" s="8" t="s">
         <v>31</v>
       </c>
-      <c r="E17" s="9"/>
-    </row>
-    <row r="18" spans="1:5" ht="13.8" x14ac:dyDescent="0.25">
-      <c r="A18" s="8" t="s">
+      <c r="E17" s="8"/>
+    </row>
+    <row r="18" spans="1:5" ht="14.25" x14ac:dyDescent="0.2">
+      <c r="A18" s="7" t="s">
         <v>32</v>
       </c>
-      <c r="B18" s="8" t="s">
+      <c r="B18" s="7" t="s">
         <v>14</v>
       </c>
-      <c r="C18" s="8" t="s">
+      <c r="C18" s="7" t="s">
         <v>15</v>
       </c>
-      <c r="D18" s="9" t="s">
+      <c r="D18" s="8" t="s">
         <v>33</v>
       </c>
-      <c r="E18" s="9"/>
-    </row>
-    <row r="19" spans="1:5" ht="27.6" x14ac:dyDescent="0.25">
-      <c r="A19" s="8" t="s">
+      <c r="E18" s="8"/>
+    </row>
+    <row r="19" spans="1:5" ht="28.5" x14ac:dyDescent="0.2">
+      <c r="A19" s="14" t="s">
         <v>34</v>
       </c>
-      <c r="B19" s="8" t="s">
+      <c r="B19" s="7" t="s">
         <v>14</v>
       </c>
-      <c r="C19" s="8"/>
-      <c r="D19" s="9" t="s">
+      <c r="C19" s="7"/>
+      <c r="D19" s="8" t="s">
         <v>35</v>
       </c>
-      <c r="E19" s="9"/>
-    </row>
-    <row r="20" spans="1:5" ht="41.4" x14ac:dyDescent="0.25">
-      <c r="A20" s="15" t="s">
+      <c r="E19" s="8"/>
+    </row>
+    <row r="20" spans="1:5" ht="42.75" x14ac:dyDescent="0.2">
+      <c r="A20" s="7" t="s">
         <v>36</v>
       </c>
-      <c r="B20" s="8" t="s">
+      <c r="B20" s="7" t="s">
         <v>37</v>
       </c>
-      <c r="C20" s="8"/>
-      <c r="D20" s="9" t="s">
+      <c r="C20" s="7"/>
+      <c r="D20" s="8" t="s">
         <v>38</v>
       </c>
-      <c r="E20" s="9"/>
-    </row>
-    <row r="21" spans="1:5" ht="13.8" x14ac:dyDescent="0.25">
-      <c r="A21" s="15" t="s">
+      <c r="E20" s="8"/>
+    </row>
+    <row r="21" spans="1:5" ht="14.25" x14ac:dyDescent="0.2">
+      <c r="A21" s="14" t="s">
         <v>39</v>
       </c>
-      <c r="B21" s="8" t="s">
+      <c r="B21" s="7" t="s">
         <v>14</v>
       </c>
-      <c r="C21" s="8"/>
-      <c r="D21" s="9" t="s">
+      <c r="C21" s="7"/>
+      <c r="D21" s="8" t="s">
         <v>40</v>
       </c>
-      <c r="E21" s="9"/>
-    </row>
-    <row r="22" spans="1:5" ht="13.8" x14ac:dyDescent="0.25">
-      <c r="A22" s="8" t="s">
+      <c r="E21" s="8"/>
+    </row>
+    <row r="22" spans="1:5" ht="14.25" x14ac:dyDescent="0.2">
+      <c r="A22" s="14" t="s">
         <v>41</v>
       </c>
-      <c r="B22" s="8" t="s">
+      <c r="B22" s="7" t="s">
         <v>14</v>
       </c>
-      <c r="C22" s="8"/>
-      <c r="D22" s="9" t="s">
+      <c r="C22" s="7"/>
+      <c r="D22" s="8" t="s">
         <v>42</v>
       </c>
-      <c r="E22" s="9"/>
-    </row>
-    <row r="23" spans="1:5" ht="13.8" x14ac:dyDescent="0.25">
-      <c r="A23" s="8" t="s">
+      <c r="E22" s="8"/>
+    </row>
+    <row r="23" spans="1:5" ht="14.25" x14ac:dyDescent="0.2">
+      <c r="A23" s="7" t="s">
         <v>43</v>
       </c>
-      <c r="B23" s="8"/>
-      <c r="C23" s="8"/>
-      <c r="D23" s="9"/>
-      <c r="E23" s="9"/>
-    </row>
-    <row r="24" spans="1:5" ht="13.8" x14ac:dyDescent="0.25">
-      <c r="A24" s="8" t="s">
+      <c r="B23" s="7"/>
+      <c r="C23" s="7"/>
+      <c r="D23" s="8"/>
+      <c r="E23" s="8"/>
+    </row>
+    <row r="24" spans="1:5" ht="14.25" x14ac:dyDescent="0.2">
+      <c r="A24" s="7" t="s">
         <v>44</v>
       </c>
-      <c r="B24" s="8"/>
-      <c r="C24" s="8"/>
-      <c r="D24" s="9"/>
-      <c r="E24" s="9"/>
-    </row>
-    <row r="25" spans="1:5" ht="27.6" x14ac:dyDescent="0.25">
-      <c r="A25" s="8" t="s">
+      <c r="B24" s="7"/>
+      <c r="C24" s="7"/>
+      <c r="D24" s="8"/>
+      <c r="E24" s="8"/>
+    </row>
+    <row r="25" spans="1:5" ht="28.5" x14ac:dyDescent="0.2">
+      <c r="A25" s="7" t="s">
         <v>45</v>
       </c>
-      <c r="B25" s="8"/>
-      <c r="C25" s="8"/>
-      <c r="D25" s="9" t="s">
+      <c r="B25" s="7"/>
+      <c r="C25" s="7"/>
+      <c r="D25" s="8" t="s">
         <v>46</v>
       </c>
-      <c r="E25" s="9"/>
-    </row>
-    <row r="26" spans="1:5" ht="13.8" x14ac:dyDescent="0.25">
-      <c r="A26" s="15" t="s">
+      <c r="E25" s="8"/>
+    </row>
+    <row r="26" spans="1:5" ht="14.25" x14ac:dyDescent="0.2">
+      <c r="A26" s="7" t="s">
         <v>47</v>
       </c>
-      <c r="B26" s="8" t="s">
+      <c r="B26" s="7" t="s">
         <v>48</v>
       </c>
-      <c r="C26" s="8"/>
-      <c r="D26" s="9"/>
-      <c r="E26" s="9"/>
-    </row>
-    <row r="27" spans="1:5" ht="13.8" x14ac:dyDescent="0.25">
-      <c r="A27" s="8" t="s">
+      <c r="C26" s="7"/>
+      <c r="D26" s="8"/>
+      <c r="E26" s="8"/>
+    </row>
+    <row r="27" spans="1:5" ht="14.25" x14ac:dyDescent="0.2">
+      <c r="A27" s="7" t="s">
         <v>49</v>
       </c>
-      <c r="B27" s="8" t="s">
+      <c r="B27" s="7" t="s">
         <v>14</v>
       </c>
-      <c r="C27" s="8"/>
-      <c r="D27" s="9"/>
-      <c r="E27" s="9"/>
-    </row>
-    <row r="28" spans="1:5" ht="13.8" x14ac:dyDescent="0.25">
-      <c r="A28" s="8" t="s">
+      <c r="C27" s="7"/>
+      <c r="D27" s="8"/>
+      <c r="E27" s="8"/>
+    </row>
+    <row r="28" spans="1:5" ht="14.25" x14ac:dyDescent="0.2">
+      <c r="A28" s="7" t="s">
         <v>50</v>
       </c>
-      <c r="B28" s="8" t="s">
+      <c r="B28" s="7" t="s">
         <v>14</v>
       </c>
-      <c r="C28" s="8"/>
-      <c r="D28" s="9"/>
-      <c r="E28" s="9"/>
-    </row>
-    <row r="29" spans="1:5" ht="13.8" x14ac:dyDescent="0.25">
-      <c r="A29" s="8" t="s">
+      <c r="C28" s="7"/>
+      <c r="D28" s="8"/>
+      <c r="E28" s="8"/>
+    </row>
+    <row r="29" spans="1:5" ht="14.25" x14ac:dyDescent="0.2">
+      <c r="A29" s="7" t="s">
         <v>51</v>
       </c>
-      <c r="B29" s="8" t="s">
+      <c r="B29" s="7" t="s">
         <v>14</v>
       </c>
-      <c r="C29" s="8"/>
-      <c r="D29" s="9"/>
-      <c r="E29" s="9"/>
-    </row>
-    <row r="30" spans="1:5" ht="27.6" x14ac:dyDescent="0.25">
-      <c r="A30" s="15" t="s">
+      <c r="C29" s="7"/>
+      <c r="D29" s="8"/>
+      <c r="E29" s="8"/>
+    </row>
+    <row r="30" spans="1:5" ht="28.5" x14ac:dyDescent="0.2">
+      <c r="A30" s="7" t="s">
         <v>52</v>
       </c>
-      <c r="B30" s="8" t="s">
+      <c r="B30" s="7" t="s">
         <v>14</v>
       </c>
-      <c r="C30" s="8"/>
-      <c r="D30" s="9" t="s">
+      <c r="C30" s="7"/>
+      <c r="D30" s="8" t="s">
         <v>53</v>
       </c>
-      <c r="E30" s="9"/>
-    </row>
-    <row r="31" spans="1:5" ht="27.6" x14ac:dyDescent="0.25">
-      <c r="A31" s="8" t="s">
+      <c r="E30" s="8"/>
+    </row>
+    <row r="31" spans="1:5" ht="28.5" x14ac:dyDescent="0.2">
+      <c r="A31" s="7" t="s">
         <v>54</v>
       </c>
-      <c r="B31" s="8" t="s">
+      <c r="B31" s="7" t="s">
         <v>14</v>
       </c>
-      <c r="C31" s="8"/>
-      <c r="D31" s="9" t="s">
+      <c r="C31" s="7"/>
+      <c r="D31" s="8" t="s">
         <v>53</v>
       </c>
-      <c r="E31" s="9"/>
-    </row>
-    <row r="32" spans="1:5" ht="13.8" x14ac:dyDescent="0.25">
-      <c r="A32" s="8" t="s">
+      <c r="E31" s="8"/>
+    </row>
+    <row r="32" spans="1:5" ht="14.25" x14ac:dyDescent="0.2">
+      <c r="A32" s="7" t="s">
         <v>55</v>
       </c>
-      <c r="B32" s="8"/>
-      <c r="C32" s="8"/>
-      <c r="D32" s="9"/>
-      <c r="E32" s="9"/>
-    </row>
-    <row r="33" spans="1:5" ht="13.8" x14ac:dyDescent="0.25">
-      <c r="A33" s="15" t="s">
+      <c r="B32" s="7"/>
+      <c r="C32" s="7"/>
+      <c r="D32" s="8"/>
+      <c r="E32" s="8"/>
+    </row>
+    <row r="33" spans="1:5" ht="14.25" x14ac:dyDescent="0.2">
+      <c r="A33" s="7" t="s">
         <v>56</v>
       </c>
-      <c r="B33" s="8" t="s">
+      <c r="B33" s="7" t="s">
         <v>48</v>
       </c>
-      <c r="C33" s="8"/>
-      <c r="D33" s="9"/>
-      <c r="E33" s="9"/>
-    </row>
-    <row r="34" spans="1:5" ht="13.8" x14ac:dyDescent="0.25">
-      <c r="A34" s="15" t="s">
+      <c r="C33" s="7"/>
+      <c r="D33" s="8"/>
+      <c r="E33" s="8"/>
+    </row>
+    <row r="34" spans="1:5" ht="14.25" x14ac:dyDescent="0.2">
+      <c r="A34" s="7" t="s">
         <v>57</v>
       </c>
-      <c r="B34" s="8" t="s">
+      <c r="B34" s="7" t="s">
         <v>48</v>
       </c>
-      <c r="C34" s="8"/>
-      <c r="D34" s="9"/>
-      <c r="E34" s="9"/>
-    </row>
-    <row r="35" spans="1:5" ht="13.8" x14ac:dyDescent="0.25">
-      <c r="A35" s="8" t="s">
+      <c r="C34" s="7"/>
+      <c r="D34" s="8"/>
+      <c r="E34" s="8"/>
+    </row>
+    <row r="35" spans="1:5" ht="14.25" x14ac:dyDescent="0.2">
+      <c r="A35" s="7" t="s">
         <v>58</v>
       </c>
-      <c r="B35" s="8" t="s">
+      <c r="B35" s="7" t="s">
         <v>14</v>
       </c>
-      <c r="C35" s="8"/>
-      <c r="D35" s="9"/>
-      <c r="E35" s="9"/>
-    </row>
-    <row r="36" spans="1:5" ht="41.4" x14ac:dyDescent="0.25">
-      <c r="A36" s="8" t="s">
+      <c r="C35" s="7"/>
+      <c r="D35" s="8"/>
+      <c r="E35" s="8"/>
+    </row>
+    <row r="36" spans="1:5" ht="57" x14ac:dyDescent="0.2">
+      <c r="A36" s="14" t="s">
         <v>59</v>
       </c>
-      <c r="B36" s="8" t="s">
+      <c r="B36" s="7" t="s">
         <v>14</v>
       </c>
-      <c r="C36" s="8" t="s">
+      <c r="C36" s="7" t="s">
         <v>15</v>
       </c>
-      <c r="D36" s="9" t="s">
+      <c r="D36" s="8" t="s">
         <v>60</v>
       </c>
-      <c r="E36" s="9"/>
-    </row>
-    <row r="37" spans="1:5" ht="55.2" x14ac:dyDescent="0.25">
-      <c r="A37" s="8" t="s">
+      <c r="E36" s="8"/>
+    </row>
+    <row r="37" spans="1:5" ht="57" x14ac:dyDescent="0.2">
+      <c r="A37" s="7" t="s">
         <v>61</v>
       </c>
-      <c r="B37" s="8" t="s">
+      <c r="B37" s="7" t="s">
         <v>14</v>
       </c>
-      <c r="C37" s="8" t="s">
+      <c r="C37" s="7" t="s">
         <v>15</v>
       </c>
-      <c r="D37" s="9" t="s">
+      <c r="D37" s="8" t="s">
         <v>62</v>
       </c>
-      <c r="E37" s="9"/>
-    </row>
-    <row r="38" spans="1:5" ht="27.6" x14ac:dyDescent="0.25">
-      <c r="A38" s="15" t="s">
+      <c r="E37" s="8"/>
+    </row>
+    <row r="38" spans="1:5" ht="28.5" x14ac:dyDescent="0.2">
+      <c r="A38" s="7" t="s">
         <v>63</v>
       </c>
-      <c r="B38" s="8" t="s">
+      <c r="B38" s="7" t="s">
         <v>64</v>
       </c>
-      <c r="C38" s="8"/>
-      <c r="D38" s="9" t="s">
+      <c r="C38" s="7"/>
+      <c r="D38" s="8" t="s">
         <v>65</v>
       </c>
-      <c r="E38" s="9"/>
-    </row>
-    <row r="39" spans="1:5" ht="27.6" x14ac:dyDescent="0.25">
-      <c r="A39" s="15" t="s">
+      <c r="E38" s="8"/>
+    </row>
+    <row r="39" spans="1:5" ht="28.5" x14ac:dyDescent="0.2">
+      <c r="A39" s="7" t="s">
         <v>66</v>
       </c>
-      <c r="B39" s="8" t="s">
+      <c r="B39" s="7" t="s">
         <v>64</v>
       </c>
-      <c r="C39" s="8"/>
-      <c r="D39" s="9" t="s">
+      <c r="C39" s="7"/>
+      <c r="D39" s="8" t="s">
         <v>65</v>
       </c>
-      <c r="E39" s="9"/>
-    </row>
-    <row r="40" spans="1:5" ht="41.4" x14ac:dyDescent="0.25">
-      <c r="A40" s="8" t="s">
+      <c r="E39" s="8"/>
+    </row>
+    <row r="40" spans="1:5" ht="42.75" x14ac:dyDescent="0.2">
+      <c r="A40" s="14" t="s">
         <v>67</v>
       </c>
-      <c r="B40" s="8" t="s">
+      <c r="B40" s="7" t="s">
         <v>14</v>
       </c>
-      <c r="C40" s="8"/>
-      <c r="D40" s="9" t="s">
+      <c r="C40" s="7"/>
+      <c r="D40" s="8" t="s">
         <v>68</v>
       </c>
-      <c r="E40" s="9"/>
-    </row>
-    <row r="41" spans="1:5" ht="409.6" x14ac:dyDescent="0.25">
-      <c r="A41" s="15" t="s">
+      <c r="E40" s="8"/>
+    </row>
+    <row r="41" spans="1:5" ht="409.5" x14ac:dyDescent="0.2">
+      <c r="A41" s="14" t="s">
         <v>69</v>
       </c>
-      <c r="B41" s="8" t="s">
+      <c r="B41" s="7" t="s">
         <v>14</v>
       </c>
-      <c r="C41" s="8"/>
-      <c r="D41" s="9" t="s">
+      <c r="C41" s="7"/>
+      <c r="D41" s="8" t="s">
         <v>70</v>
       </c>
-      <c r="E41" s="10" t="s">
+      <c r="E41" s="9" t="s">
         <v>71</v>
       </c>
     </row>
-    <row r="42" spans="1:5" ht="13.8" x14ac:dyDescent="0.25">
-      <c r="A42" s="15" t="s">
+    <row r="42" spans="1:5" ht="14.25" x14ac:dyDescent="0.2">
+      <c r="A42" s="7" t="s">
         <v>72</v>
       </c>
-      <c r="B42" s="8" t="s">
+      <c r="B42" s="7" t="s">
         <v>11</v>
       </c>
-      <c r="C42" s="8"/>
-      <c r="D42" s="9" t="s">
+      <c r="C42" s="7"/>
+      <c r="D42" s="8" t="s">
         <v>73</v>
       </c>
-      <c r="E42" s="9"/>
-    </row>
-    <row r="43" spans="1:5" ht="13.8" x14ac:dyDescent="0.25">
-      <c r="A43" s="15" t="s">
+      <c r="E42" s="8"/>
+    </row>
+    <row r="43" spans="1:5" ht="14.25" x14ac:dyDescent="0.2">
+      <c r="A43" s="7" t="s">
         <v>74</v>
       </c>
-      <c r="B43" s="8" t="s">
+      <c r="B43" s="7" t="s">
         <v>64</v>
       </c>
-      <c r="C43" s="8"/>
-      <c r="D43" s="9" t="s">
+      <c r="C43" s="7"/>
+      <c r="D43" s="8" t="s">
         <v>75</v>
       </c>
-      <c r="E43" s="9"/>
-    </row>
-    <row r="44" spans="1:5" ht="69" x14ac:dyDescent="0.25">
-      <c r="A44" s="8" t="s">
+      <c r="E43" s="8"/>
+    </row>
+    <row r="44" spans="1:5" ht="71.25" x14ac:dyDescent="0.2">
+      <c r="A44" s="7" t="s">
         <v>76</v>
       </c>
-      <c r="B44" s="8" t="s">
+      <c r="B44" s="7" t="s">
         <v>77</v>
       </c>
-      <c r="C44" s="8"/>
-      <c r="D44" s="9" t="s">
+      <c r="C44" s="7"/>
+      <c r="D44" s="8" t="s">
         <v>78</v>
       </c>
-      <c r="E44" s="9"/>
-    </row>
-    <row r="45" spans="1:5" ht="13.8" x14ac:dyDescent="0.25">
-      <c r="A45" s="15" t="s">
+      <c r="E44" s="8"/>
+    </row>
+    <row r="45" spans="1:5" ht="14.25" x14ac:dyDescent="0.2">
+      <c r="A45" s="7" t="s">
         <v>79</v>
       </c>
-      <c r="B45" s="8" t="s">
+      <c r="B45" s="7" t="s">
         <v>11</v>
       </c>
-      <c r="C45" s="8"/>
-      <c r="D45" s="9" t="s">
+      <c r="C45" s="7"/>
+      <c r="D45" s="8" t="s">
         <v>80</v>
       </c>
-      <c r="E45" s="9"/>
-    </row>
-    <row r="46" spans="1:5" ht="13.8" x14ac:dyDescent="0.25">
-      <c r="A46" s="15" t="s">
+      <c r="E45" s="8"/>
+    </row>
+    <row r="46" spans="1:5" ht="14.25" x14ac:dyDescent="0.2">
+      <c r="A46" s="7" t="s">
         <v>81</v>
       </c>
-      <c r="B46" s="8" t="s">
+      <c r="B46" s="7" t="s">
         <v>11</v>
       </c>
-      <c r="C46" s="8"/>
-      <c r="D46" s="9" t="s">
+      <c r="C46" s="7"/>
+      <c r="D46" s="8" t="s">
         <v>82</v>
       </c>
-      <c r="E46" s="9"/>
-    </row>
-    <row r="47" spans="1:5" ht="13.8" x14ac:dyDescent="0.25">
-      <c r="A47" s="8" t="s">
+      <c r="E46" s="8"/>
+    </row>
+    <row r="47" spans="1:5" ht="14.25" x14ac:dyDescent="0.2">
+      <c r="A47" s="14" t="s">
         <v>83</v>
       </c>
-      <c r="B47" s="8" t="s">
+      <c r="B47" s="7" t="s">
         <v>84</v>
       </c>
-      <c r="C47" s="8"/>
-      <c r="D47" s="9"/>
-      <c r="E47" s="9"/>
-    </row>
-    <row r="48" spans="1:5" ht="13.8" x14ac:dyDescent="0.25">
-      <c r="A48" s="15" t="s">
+      <c r="C47" s="7"/>
+      <c r="D47" s="8"/>
+      <c r="E47" s="8"/>
+    </row>
+    <row r="48" spans="1:5" ht="14.25" x14ac:dyDescent="0.2">
+      <c r="A48" s="14" t="s">
         <v>85</v>
       </c>
-      <c r="B48" s="8" t="s">
+      <c r="B48" s="7" t="s">
         <v>86</v>
       </c>
-      <c r="C48" s="8"/>
-      <c r="D48" s="9" t="s">
+      <c r="C48" s="7"/>
+      <c r="D48" s="8" t="s">
         <v>87</v>
       </c>
-      <c r="E48" s="9"/>
-    </row>
-    <row r="49" spans="1:5" ht="27.6" x14ac:dyDescent="0.25">
-      <c r="A49" s="8" t="s">
+      <c r="E48" s="8"/>
+    </row>
+    <row r="49" spans="1:5" ht="28.5" x14ac:dyDescent="0.2">
+      <c r="A49" s="7" t="s">
         <v>88</v>
       </c>
-      <c r="B49" s="8" t="s">
+      <c r="B49" s="7" t="s">
         <v>11</v>
       </c>
-      <c r="C49" s="8"/>
-      <c r="D49" s="9" t="s">
+      <c r="C49" s="7"/>
+      <c r="D49" s="8" t="s">
         <v>89</v>
       </c>
-      <c r="E49" s="9"/>
-    </row>
-    <row r="50" spans="1:5" ht="27.6" x14ac:dyDescent="0.25">
-      <c r="A50" s="8" t="s">
+      <c r="E49" s="8"/>
+    </row>
+    <row r="50" spans="1:5" ht="28.5" x14ac:dyDescent="0.2">
+      <c r="A50" s="7" t="s">
         <v>90</v>
       </c>
-      <c r="B50" s="8" t="s">
+      <c r="B50" s="7" t="s">
         <v>11</v>
       </c>
-      <c r="C50" s="8"/>
-      <c r="D50" s="9" t="s">
+      <c r="C50" s="7"/>
+      <c r="D50" s="8" t="s">
         <v>91</v>
       </c>
-      <c r="E50" s="9"/>
-    </row>
-    <row r="51" spans="1:5" ht="27.6" x14ac:dyDescent="0.25">
-      <c r="A51" s="8" t="s">
+      <c r="E50" s="8"/>
+    </row>
+    <row r="51" spans="1:5" ht="28.5" x14ac:dyDescent="0.2">
+      <c r="A51" s="7" t="s">
         <v>92</v>
       </c>
-      <c r="B51" s="8" t="s">
+      <c r="B51" s="7" t="s">
         <v>11</v>
       </c>
-      <c r="C51" s="8" t="s">
+      <c r="C51" s="7" t="s">
         <v>15</v>
       </c>
-      <c r="D51" s="9" t="s">
+      <c r="D51" s="8" t="s">
         <v>93</v>
       </c>
-      <c r="E51" s="9"/>
-    </row>
-    <row r="52" spans="1:5" ht="27.6" x14ac:dyDescent="0.25">
-      <c r="A52" s="8" t="s">
+      <c r="E51" s="8"/>
+    </row>
+    <row r="52" spans="1:5" ht="28.5" x14ac:dyDescent="0.2">
+      <c r="A52" s="7" t="s">
         <v>94</v>
       </c>
-      <c r="B52" s="8" t="s">
+      <c r="B52" s="7" t="s">
         <v>11</v>
       </c>
-      <c r="C52" s="8" t="s">
+      <c r="C52" s="7" t="s">
         <v>15</v>
       </c>
-      <c r="D52" s="9" t="s">
+      <c r="D52" s="8" t="s">
         <v>95</v>
       </c>
-      <c r="E52" s="9"/>
-    </row>
-    <row r="53" spans="1:5" ht="27.6" x14ac:dyDescent="0.25">
-      <c r="A53" s="8" t="s">
+      <c r="E52" s="8"/>
+    </row>
+    <row r="53" spans="1:5" ht="28.5" x14ac:dyDescent="0.2">
+      <c r="A53" s="7" t="s">
         <v>96</v>
       </c>
-      <c r="B53" s="8" t="s">
+      <c r="B53" s="7" t="s">
         <v>11</v>
       </c>
-      <c r="C53" s="8" t="s">
+      <c r="C53" s="7" t="s">
         <v>15</v>
       </c>
-      <c r="D53" s="9" t="s">
+      <c r="D53" s="8" t="s">
         <v>97</v>
       </c>
-      <c r="E53" s="9"/>
-    </row>
-    <row r="54" spans="1:5" ht="27.6" x14ac:dyDescent="0.25">
-      <c r="A54" s="8" t="s">
+      <c r="E53" s="8"/>
+    </row>
+    <row r="54" spans="1:5" ht="28.5" x14ac:dyDescent="0.2">
+      <c r="A54" s="7" t="s">
         <v>98</v>
       </c>
-      <c r="B54" s="8" t="s">
+      <c r="B54" s="7" t="s">
         <v>11</v>
       </c>
-      <c r="C54" s="8" t="s">
+      <c r="C54" s="7" t="s">
         <v>15</v>
       </c>
-      <c r="D54" s="9" t="s">
+      <c r="D54" s="8" t="s">
         <v>99</v>
       </c>
-      <c r="E54" s="9"/>
-    </row>
-    <row r="55" spans="1:5" ht="27.6" x14ac:dyDescent="0.25">
-      <c r="A55" s="8" t="s">
+      <c r="E54" s="8"/>
+    </row>
+    <row r="55" spans="1:5" ht="28.5" x14ac:dyDescent="0.2">
+      <c r="A55" s="7" t="s">
         <v>100</v>
       </c>
-      <c r="B55" s="8" t="s">
+      <c r="B55" s="7" t="s">
         <v>64</v>
       </c>
-      <c r="C55" s="8" t="s">
+      <c r="C55" s="7" t="s">
         <v>15</v>
       </c>
-      <c r="D55" s="9" t="s">
+      <c r="D55" s="8" t="s">
         <v>101</v>
       </c>
-      <c r="E55" s="9"/>
-    </row>
-    <row r="56" spans="1:5" ht="27.6" x14ac:dyDescent="0.25">
-      <c r="A56" s="8" t="s">
+      <c r="E55" s="8"/>
+    </row>
+    <row r="56" spans="1:5" ht="28.5" x14ac:dyDescent="0.2">
+      <c r="A56" s="7" t="s">
         <v>102</v>
       </c>
-      <c r="B56" s="8" t="s">
+      <c r="B56" s="7" t="s">
         <v>64</v>
       </c>
-      <c r="C56" s="8" t="s">
+      <c r="C56" s="7" t="s">
         <v>15</v>
       </c>
-      <c r="D56" s="9" t="s">
+      <c r="D56" s="8" t="s">
         <v>103</v>
       </c>
-      <c r="E56" s="9"/>
-    </row>
-    <row r="57" spans="1:5" ht="13.8" x14ac:dyDescent="0.25">
-      <c r="A57" s="8" t="s">
+      <c r="E56" s="8"/>
+    </row>
+    <row r="57" spans="1:5" ht="14.25" x14ac:dyDescent="0.2">
+      <c r="A57" s="7" t="s">
         <v>104</v>
       </c>
-      <c r="B57" s="8" t="s">
+      <c r="B57" s="7" t="s">
         <v>37</v>
       </c>
-      <c r="C57" s="8"/>
-      <c r="D57" s="9"/>
-      <c r="E57" s="9"/>
-    </row>
-    <row r="58" spans="1:5" ht="13.8" x14ac:dyDescent="0.25">
-      <c r="A58" s="8" t="s">
+      <c r="C57" s="7"/>
+      <c r="D57" s="8"/>
+      <c r="E57" s="8"/>
+    </row>
+    <row r="58" spans="1:5" ht="14.25" x14ac:dyDescent="0.2">
+      <c r="A58" s="7" t="s">
         <v>105</v>
       </c>
-      <c r="B58" s="8" t="s">
+      <c r="B58" s="7" t="s">
         <v>106</v>
       </c>
-      <c r="C58" s="8"/>
-      <c r="D58" s="9" t="s">
+      <c r="C58" s="7"/>
+      <c r="D58" s="8" t="s">
         <v>107</v>
       </c>
-      <c r="E58" s="9"/>
-    </row>
-    <row r="59" spans="1:5" ht="69" x14ac:dyDescent="0.25">
-      <c r="A59" s="15" t="s">
+      <c r="E58" s="8"/>
+    </row>
+    <row r="59" spans="1:5" ht="71.25" x14ac:dyDescent="0.2">
+      <c r="A59" s="7" t="s">
         <v>108</v>
       </c>
-      <c r="B59" s="8" t="s">
+      <c r="B59" s="7" t="s">
         <v>11</v>
       </c>
-      <c r="C59" s="8" t="s">
+      <c r="C59" s="7" t="s">
         <v>15</v>
       </c>
-      <c r="D59" s="9" t="s">
+      <c r="D59" s="8" t="s">
         <v>109</v>
       </c>
-      <c r="E59" s="9"/>
-    </row>
-    <row r="60" spans="1:5" ht="69" x14ac:dyDescent="0.25">
-      <c r="A60" s="15" t="s">
+      <c r="E59" s="8"/>
+    </row>
+    <row r="60" spans="1:5" ht="71.25" x14ac:dyDescent="0.2">
+      <c r="A60" s="7" t="s">
         <v>110</v>
       </c>
-      <c r="B60" s="8" t="s">
+      <c r="B60" s="7" t="s">
         <v>11</v>
       </c>
-      <c r="C60" s="8" t="s">
+      <c r="C60" s="7" t="s">
         <v>15</v>
       </c>
-      <c r="D60" s="9" t="s">
+      <c r="D60" s="8" t="s">
         <v>109</v>
       </c>
-      <c r="E60" s="9"/>
-    </row>
-    <row r="61" spans="1:5" ht="69" x14ac:dyDescent="0.25">
-      <c r="A61" s="15" t="s">
+      <c r="E60" s="8"/>
+    </row>
+    <row r="61" spans="1:5" ht="71.25" x14ac:dyDescent="0.2">
+      <c r="A61" s="7" t="s">
         <v>111</v>
       </c>
-      <c r="B61" s="8" t="s">
+      <c r="B61" s="7" t="s">
         <v>11</v>
       </c>
-      <c r="C61" s="8" t="s">
+      <c r="C61" s="7" t="s">
         <v>15</v>
       </c>
-      <c r="D61" s="9" t="s">
+      <c r="D61" s="8" t="s">
         <v>109</v>
       </c>
-      <c r="E61" s="9"/>
-    </row>
-    <row r="62" spans="1:5" ht="69" x14ac:dyDescent="0.25">
-      <c r="A62" s="15" t="s">
+      <c r="E61" s="8"/>
+    </row>
+    <row r="62" spans="1:5" ht="71.25" x14ac:dyDescent="0.2">
+      <c r="A62" s="7" t="s">
         <v>112</v>
       </c>
-      <c r="B62" s="8" t="s">
+      <c r="B62" s="7" t="s">
         <v>11</v>
       </c>
-      <c r="C62" s="8" t="s">
+      <c r="C62" s="7" t="s">
         <v>15</v>
       </c>
-      <c r="D62" s="9" t="s">
+      <c r="D62" s="8" t="s">
         <v>109</v>
       </c>
-      <c r="E62" s="9"/>
-    </row>
-    <row r="63" spans="1:5" ht="13.8" x14ac:dyDescent="0.25">
-      <c r="A63" s="8" t="s">
+      <c r="E62" s="8"/>
+    </row>
+    <row r="63" spans="1:5" ht="14.25" x14ac:dyDescent="0.2">
+      <c r="A63" s="7" t="s">
         <v>113</v>
       </c>
-      <c r="B63" s="8" t="s">
+      <c r="B63" s="7" t="s">
         <v>37</v>
       </c>
-      <c r="C63" s="8"/>
-      <c r="D63" s="9"/>
-      <c r="E63" s="9"/>
-    </row>
-    <row r="64" spans="1:5" ht="13.8" x14ac:dyDescent="0.25">
-      <c r="A64" s="15" t="s">
+      <c r="C63" s="7"/>
+      <c r="D63" s="8"/>
+      <c r="E63" s="8"/>
+    </row>
+    <row r="64" spans="1:5" ht="14.25" x14ac:dyDescent="0.2">
+      <c r="A64" s="7" t="s">
         <v>114</v>
       </c>
-      <c r="B64" s="8" t="s">
+      <c r="B64" s="7" t="s">
         <v>11</v>
       </c>
-      <c r="C64" s="8"/>
-      <c r="D64" s="9" t="s">
+      <c r="C64" s="7"/>
+      <c r="D64" s="8" t="s">
         <v>115</v>
       </c>
-      <c r="E64" s="9"/>
-    </row>
-    <row r="65" spans="1:5" ht="27.6" x14ac:dyDescent="0.25">
-      <c r="A65" s="15" t="s">
+      <c r="E64" s="8"/>
+    </row>
+    <row r="65" spans="1:5" ht="28.5" x14ac:dyDescent="0.2">
+      <c r="A65" s="7" t="s">
         <v>116</v>
       </c>
-      <c r="B65" s="8" t="s">
+      <c r="B65" s="7" t="s">
         <v>11</v>
       </c>
-      <c r="C65" s="8" t="s">
+      <c r="C65" s="7" t="s">
         <v>15</v>
       </c>
-      <c r="D65" s="9" t="s">
+      <c r="D65" s="8" t="s">
         <v>117</v>
       </c>
-      <c r="E65" s="9"/>
-    </row>
-    <row r="66" spans="1:5" ht="27.6" x14ac:dyDescent="0.25">
-      <c r="A66" s="15" t="s">
+      <c r="E65" s="8"/>
+    </row>
+    <row r="66" spans="1:5" ht="28.5" x14ac:dyDescent="0.2">
+      <c r="A66" s="7" t="s">
         <v>118</v>
       </c>
-      <c r="B66" s="8" t="s">
+      <c r="B66" s="7" t="s">
         <v>11</v>
       </c>
-      <c r="C66" s="8" t="s">
+      <c r="C66" s="7" t="s">
         <v>15</v>
       </c>
-      <c r="D66" s="9" t="s">
+      <c r="D66" s="8" t="s">
         <v>119</v>
       </c>
-      <c r="E66" s="9"/>
-    </row>
-    <row r="67" spans="1:5" ht="13.8" x14ac:dyDescent="0.25">
-      <c r="A67" s="8" t="s">
+      <c r="E66" s="8"/>
+    </row>
+    <row r="67" spans="1:5" ht="14.25" x14ac:dyDescent="0.2">
+      <c r="A67" s="7" t="s">
         <v>120</v>
       </c>
-      <c r="B67" s="8" t="s">
+      <c r="B67" s="7" t="s">
         <v>37</v>
       </c>
-      <c r="C67" s="8" t="s">
+      <c r="C67" s="7" t="s">
         <v>15</v>
       </c>
-      <c r="D67" s="9" t="s">
+      <c r="D67" s="8" t="s">
         <v>121</v>
       </c>
-      <c r="E67" s="9"/>
-    </row>
-    <row r="68" spans="1:5" ht="13.8" x14ac:dyDescent="0.25">
-      <c r="A68" s="8" t="s">
+      <c r="E67" s="8"/>
+    </row>
+    <row r="68" spans="1:5" ht="14.25" x14ac:dyDescent="0.2">
+      <c r="A68" s="7" t="s">
         <v>122</v>
       </c>
-      <c r="B68" s="8" t="s">
+      <c r="B68" s="7" t="s">
         <v>37</v>
       </c>
-      <c r="C68" s="8" t="s">
+      <c r="C68" s="7" t="s">
         <v>15</v>
       </c>
-      <c r="D68" s="9" t="s">
+      <c r="D68" s="8" t="s">
         <v>123</v>
       </c>
-      <c r="E68" s="9"/>
-    </row>
-    <row r="69" spans="1:5" ht="13.8" x14ac:dyDescent="0.25">
-      <c r="A69" s="15" t="s">
+      <c r="E68" s="8"/>
+    </row>
+    <row r="69" spans="1:5" ht="14.25" x14ac:dyDescent="0.2">
+      <c r="A69" s="7" t="s">
         <v>124</v>
       </c>
-      <c r="B69" s="8"/>
-      <c r="C69" s="8"/>
-      <c r="D69" s="9"/>
-      <c r="E69" s="9"/>
-    </row>
-    <row r="70" spans="1:5" ht="13.8" x14ac:dyDescent="0.25">
-      <c r="A70" s="15" t="s">
+      <c r="B69" s="7"/>
+      <c r="C69" s="7"/>
+      <c r="D69" s="8"/>
+      <c r="E69" s="8"/>
+    </row>
+    <row r="70" spans="1:5" ht="14.25" x14ac:dyDescent="0.2">
+      <c r="A70" s="7" t="s">
         <v>125</v>
       </c>
-      <c r="B70" s="8"/>
-      <c r="C70" s="8"/>
-      <c r="D70" s="9"/>
-      <c r="E70" s="9"/>
-    </row>
-    <row r="71" spans="1:5" ht="13.8" x14ac:dyDescent="0.25">
-      <c r="A71" s="15" t="s">
+      <c r="B70" s="7"/>
+      <c r="C70" s="7"/>
+      <c r="D70" s="8"/>
+      <c r="E70" s="8"/>
+    </row>
+    <row r="71" spans="1:5" ht="14.25" x14ac:dyDescent="0.2">
+      <c r="A71" s="7" t="s">
         <v>126</v>
       </c>
-      <c r="B71" s="8"/>
-      <c r="C71" s="8"/>
-      <c r="D71" s="9"/>
-      <c r="E71" s="9"/>
-    </row>
-    <row r="72" spans="1:5" ht="13.8" x14ac:dyDescent="0.25">
-      <c r="A72" s="15" t="s">
+      <c r="B71" s="7"/>
+      <c r="C71" s="7"/>
+      <c r="D71" s="8"/>
+      <c r="E71" s="8"/>
+    </row>
+    <row r="72" spans="1:5" ht="14.25" x14ac:dyDescent="0.2">
+      <c r="A72" s="7" t="s">
         <v>127</v>
       </c>
-      <c r="B72" s="8"/>
-      <c r="C72" s="8"/>
-      <c r="D72" s="9"/>
-      <c r="E72" s="9"/>
-    </row>
-    <row r="73" spans="1:5" ht="13.8" x14ac:dyDescent="0.25">
-      <c r="A73" s="15" t="s">
+      <c r="B72" s="7"/>
+      <c r="C72" s="7"/>
+      <c r="D72" s="8"/>
+      <c r="E72" s="8"/>
+    </row>
+    <row r="73" spans="1:5" ht="14.25" x14ac:dyDescent="0.2">
+      <c r="A73" s="7" t="s">
         <v>128</v>
       </c>
-      <c r="B73" s="8"/>
-      <c r="C73" s="8"/>
-      <c r="D73" s="9"/>
-      <c r="E73" s="9"/>
-    </row>
-    <row r="74" spans="1:5" ht="13.8" x14ac:dyDescent="0.25">
-      <c r="A74" s="15" t="s">
+      <c r="B73" s="7"/>
+      <c r="C73" s="7"/>
+      <c r="D73" s="8"/>
+      <c r="E73" s="8"/>
+    </row>
+    <row r="74" spans="1:5" ht="14.25" x14ac:dyDescent="0.2">
+      <c r="A74" s="7" t="s">
         <v>129</v>
       </c>
-      <c r="B74" s="8"/>
-      <c r="C74" s="8"/>
-      <c r="D74" s="9"/>
-      <c r="E74" s="9"/>
-    </row>
-    <row r="75" spans="1:5" ht="13.8" x14ac:dyDescent="0.25">
-      <c r="A75" s="15" t="s">
+      <c r="B74" s="7"/>
+      <c r="C74" s="7"/>
+      <c r="D74" s="8"/>
+      <c r="E74" s="8"/>
+    </row>
+    <row r="75" spans="1:5" ht="14.25" x14ac:dyDescent="0.2">
+      <c r="A75" s="7" t="s">
         <v>130</v>
       </c>
-      <c r="B75" s="8"/>
-      <c r="C75" s="8"/>
-      <c r="D75" s="9"/>
-      <c r="E75" s="9"/>
-    </row>
-    <row r="76" spans="1:5" ht="13.8" x14ac:dyDescent="0.25">
-      <c r="A76" s="8" t="s">
+      <c r="B75" s="7"/>
+      <c r="C75" s="7"/>
+      <c r="D75" s="8"/>
+      <c r="E75" s="8"/>
+    </row>
+    <row r="76" spans="1:5" ht="14.25" x14ac:dyDescent="0.2">
+      <c r="A76" s="7" t="s">
         <v>131</v>
       </c>
-      <c r="B76" s="8" t="s">
+      <c r="B76" s="7" t="s">
         <v>14</v>
       </c>
-      <c r="C76" s="8"/>
-      <c r="D76" s="9" t="s">
+      <c r="C76" s="7"/>
+      <c r="D76" s="8" t="s">
         <v>132</v>
       </c>
-      <c r="E76" s="9"/>
-    </row>
-    <row r="77" spans="1:5" ht="55.2" x14ac:dyDescent="0.25">
-      <c r="A77" s="15" t="s">
+      <c r="E76" s="8"/>
+    </row>
+    <row r="77" spans="1:5" ht="57" x14ac:dyDescent="0.2">
+      <c r="A77" s="7" t="s">
         <v>133</v>
       </c>
-      <c r="B77" s="8" t="s">
+      <c r="B77" s="7" t="s">
         <v>106</v>
       </c>
-      <c r="C77" s="8"/>
-      <c r="D77" s="9" t="s">
+      <c r="C77" s="7"/>
+      <c r="D77" s="8" t="s">
         <v>134</v>
       </c>
-      <c r="E77" s="9"/>
-    </row>
-    <row r="78" spans="1:5" ht="27.6" x14ac:dyDescent="0.25">
-      <c r="A78" s="8" t="s">
+      <c r="E77" s="8"/>
+    </row>
+    <row r="78" spans="1:5" ht="28.5" x14ac:dyDescent="0.2">
+      <c r="A78" s="7" t="s">
         <v>135</v>
       </c>
-      <c r="B78" s="8" t="s">
+      <c r="B78" s="7" t="s">
         <v>11</v>
       </c>
-      <c r="C78" s="8" t="s">
+      <c r="C78" s="7" t="s">
         <v>15</v>
       </c>
-      <c r="D78" s="9" t="s">
+      <c r="D78" s="8" t="s">
         <v>136</v>
       </c>
-      <c r="E78" s="9"/>
-    </row>
-    <row r="79" spans="1:5" ht="41.4" x14ac:dyDescent="0.25">
-      <c r="A79" s="8" t="s">
+      <c r="E78" s="8"/>
+    </row>
+    <row r="79" spans="1:5" ht="42.75" x14ac:dyDescent="0.2">
+      <c r="A79" s="7" t="s">
         <v>137</v>
       </c>
-      <c r="B79" s="8" t="s">
+      <c r="B79" s="7" t="s">
         <v>11</v>
       </c>
-      <c r="C79" s="8" t="s">
+      <c r="C79" s="7" t="s">
         <v>15</v>
       </c>
-      <c r="D79" s="9" t="s">
+      <c r="D79" s="8" t="s">
         <v>138</v>
       </c>
-      <c r="E79" s="9"/>
-    </row>
-    <row r="80" spans="1:5" ht="41.4" x14ac:dyDescent="0.25">
-      <c r="A80" s="8" t="s">
+      <c r="E79" s="8"/>
+    </row>
+    <row r="80" spans="1:5" ht="42.75" x14ac:dyDescent="0.2">
+      <c r="A80" s="7" t="s">
         <v>139</v>
       </c>
-      <c r="B80" s="8" t="s">
+      <c r="B80" s="7" t="s">
         <v>11</v>
       </c>
-      <c r="C80" s="8" t="s">
+      <c r="C80" s="7" t="s">
         <v>15</v>
       </c>
-      <c r="D80" s="9" t="s">
+      <c r="D80" s="8" t="s">
         <v>140</v>
       </c>
-      <c r="E80" s="9"/>
-    </row>
-    <row r="81" spans="1:5" ht="41.4" x14ac:dyDescent="0.25">
-      <c r="A81" s="8" t="s">
+      <c r="E80" s="8"/>
+    </row>
+    <row r="81" spans="1:5" ht="42.75" x14ac:dyDescent="0.2">
+      <c r="A81" s="7" t="s">
         <v>141</v>
       </c>
-      <c r="B81" s="8" t="s">
+      <c r="B81" s="7" t="s">
         <v>11</v>
       </c>
-      <c r="C81" s="8" t="s">
+      <c r="C81" s="7" t="s">
         <v>15</v>
       </c>
-      <c r="D81" s="9" t="s">
+      <c r="D81" s="8" t="s">
         <v>142</v>
       </c>
-      <c r="E81" s="9"/>
-    </row>
-    <row r="82" spans="1:5" ht="27.6" x14ac:dyDescent="0.25">
-      <c r="A82" s="8" t="s">
+      <c r="E81" s="8"/>
+    </row>
+    <row r="82" spans="1:5" ht="28.5" x14ac:dyDescent="0.2">
+      <c r="A82" s="7" t="s">
         <v>143</v>
       </c>
-      <c r="B82" s="8" t="s">
+      <c r="B82" s="7" t="s">
         <v>64</v>
       </c>
-      <c r="C82" s="8" t="s">
+      <c r="C82" s="7" t="s">
         <v>15</v>
       </c>
-      <c r="D82" s="9" t="s">
+      <c r="D82" s="8" t="s">
         <v>144</v>
       </c>
-      <c r="E82" s="9"/>
-    </row>
-    <row r="84" spans="1:5" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A84" s="11" t="s">
+      <c r="E82" s="8"/>
+    </row>
+    <row r="84" spans="1:5" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A84" s="10" t="s">
         <v>145</v>
       </c>
     </row>
-    <row r="85" spans="1:5" ht="13.8" x14ac:dyDescent="0.25">
-      <c r="A85" s="12" t="s">
+    <row r="85" spans="1:5" ht="15" x14ac:dyDescent="0.25">
+      <c r="A85" s="11" t="s">
         <v>6</v>
       </c>
-      <c r="B85" s="12" t="s">
+      <c r="B85" s="11" t="s">
         <v>146</v>
       </c>
     </row>
-    <row r="86" spans="1:5" ht="13.8" x14ac:dyDescent="0.25">
-      <c r="A86" s="8" t="s">
+    <row r="86" spans="1:5" ht="14.25" x14ac:dyDescent="0.2">
+      <c r="A86" s="7" t="s">
         <v>147</v>
       </c>
-      <c r="B86" s="3" t="s">
-        <v>148</v>
-      </c>
-    </row>
-    <row r="87" spans="1:5" ht="13.8" x14ac:dyDescent="0.25">
-      <c r="A87" s="8" t="s">
+      <c r="B86" s="2" t="s">
+        <v>148</v>
+      </c>
+    </row>
+    <row r="87" spans="1:5" ht="14.25" x14ac:dyDescent="0.2">
+      <c r="A87" s="7" t="s">
         <v>149</v>
       </c>
-      <c r="B87" s="3" t="s">
-        <v>148</v>
-      </c>
-    </row>
-    <row r="88" spans="1:5" ht="13.8" x14ac:dyDescent="0.25">
-      <c r="A88" s="8" t="s">
+      <c r="B87" s="2" t="s">
+        <v>148</v>
+      </c>
+    </row>
+    <row r="88" spans="1:5" ht="14.25" x14ac:dyDescent="0.2">
+      <c r="A88" s="7" t="s">
         <v>150</v>
       </c>
-      <c r="B88" s="3" t="s">
-        <v>148</v>
-      </c>
-    </row>
-    <row r="89" spans="1:5" ht="13.8" x14ac:dyDescent="0.25">
-      <c r="A89" s="8" t="s">
+      <c r="B88" s="2" t="s">
+        <v>148</v>
+      </c>
+    </row>
+    <row r="89" spans="1:5" ht="14.25" x14ac:dyDescent="0.2">
+      <c r="A89" s="7" t="s">
         <v>151</v>
       </c>
-      <c r="B89" s="3" t="s">
-        <v>148</v>
-      </c>
-    </row>
-    <row r="90" spans="1:5" ht="13.8" x14ac:dyDescent="0.25">
-      <c r="A90" s="8" t="s">
+      <c r="B89" s="2" t="s">
+        <v>148</v>
+      </c>
+    </row>
+    <row r="90" spans="1:5" ht="14.25" x14ac:dyDescent="0.2">
+      <c r="A90" s="7" t="s">
         <v>152</v>
       </c>
-      <c r="B90" s="3" t="s">
-        <v>148</v>
-      </c>
-    </row>
-    <row r="91" spans="1:5" ht="13.8" x14ac:dyDescent="0.25">
-      <c r="A91" s="8" t="s">
+      <c r="B90" s="2" t="s">
+        <v>148</v>
+      </c>
+    </row>
+    <row r="91" spans="1:5" ht="14.25" x14ac:dyDescent="0.2">
+      <c r="A91" s="7" t="s">
         <v>153</v>
       </c>
-      <c r="B91" s="3" t="s">
-        <v>148</v>
-      </c>
-    </row>
-    <row r="92" spans="1:5" ht="13.8" x14ac:dyDescent="0.25">
-      <c r="A92" s="8" t="s">
+      <c r="B91" s="2" t="s">
+        <v>148</v>
+      </c>
+    </row>
+    <row r="92" spans="1:5" ht="14.25" x14ac:dyDescent="0.2">
+      <c r="A92" s="7" t="s">
         <v>154</v>
       </c>
-      <c r="B92" s="3" t="s">
-        <v>148</v>
-      </c>
-    </row>
-    <row r="93" spans="1:5" ht="13.8" x14ac:dyDescent="0.25">
-      <c r="A93" s="8" t="s">
+      <c r="B92" s="2" t="s">
+        <v>148</v>
+      </c>
+    </row>
+    <row r="93" spans="1:5" ht="14.25" x14ac:dyDescent="0.2">
+      <c r="A93" s="7" t="s">
         <v>155</v>
       </c>
-      <c r="B93" s="3" t="s">
-        <v>148</v>
-      </c>
-    </row>
-    <row r="94" spans="1:5" ht="13.8" x14ac:dyDescent="0.25">
-      <c r="A94" s="8" t="s">
+      <c r="B93" s="2" t="s">
+        <v>148</v>
+      </c>
+    </row>
+    <row r="94" spans="1:5" ht="14.25" x14ac:dyDescent="0.2">
+      <c r="A94" s="7" t="s">
         <v>156</v>
       </c>
-      <c r="B94" s="3" t="s">
-        <v>148</v>
-      </c>
-    </row>
-    <row r="95" spans="1:5" ht="13.8" x14ac:dyDescent="0.25">
-      <c r="A95" s="8" t="s">
+      <c r="B94" s="2" t="s">
+        <v>148</v>
+      </c>
+    </row>
+    <row r="95" spans="1:5" ht="14.25" x14ac:dyDescent="0.2">
+      <c r="A95" s="7" t="s">
         <v>157</v>
       </c>
-      <c r="B95" s="3" t="s">
-        <v>148</v>
-      </c>
-    </row>
-    <row r="96" spans="1:5" ht="13.8" x14ac:dyDescent="0.25">
-      <c r="A96" s="8" t="s">
+      <c r="B95" s="2" t="s">
+        <v>148</v>
+      </c>
+    </row>
+    <row r="96" spans="1:5" ht="14.25" x14ac:dyDescent="0.2">
+      <c r="A96" s="7" t="s">
         <v>158</v>
       </c>
-      <c r="B96" s="3" t="s">
-        <v>148</v>
-      </c>
-    </row>
-    <row r="97" spans="1:2" ht="13.8" x14ac:dyDescent="0.25">
-      <c r="A97" s="8" t="s">
+      <c r="B96" s="2" t="s">
+        <v>148</v>
+      </c>
+    </row>
+    <row r="97" spans="1:2" ht="14.25" x14ac:dyDescent="0.2">
+      <c r="A97" s="7" t="s">
         <v>159</v>
       </c>
-      <c r="B97" s="3" t="s">
-        <v>148</v>
-      </c>
-    </row>
-    <row r="98" spans="1:2" ht="13.8" x14ac:dyDescent="0.25">
-      <c r="A98" s="8" t="s">
+      <c r="B97" s="2" t="s">
+        <v>148</v>
+      </c>
+    </row>
+    <row r="98" spans="1:2" ht="14.25" x14ac:dyDescent="0.2">
+      <c r="A98" s="7" t="s">
         <v>160</v>
       </c>
-      <c r="B98" s="3" t="s">
-        <v>148</v>
-      </c>
-    </row>
-    <row r="99" spans="1:2" ht="13.8" x14ac:dyDescent="0.25">
-      <c r="A99" s="8" t="s">
+      <c r="B98" s="2" t="s">
+        <v>148</v>
+      </c>
+    </row>
+    <row r="99" spans="1:2" ht="14.25" x14ac:dyDescent="0.2">
+      <c r="A99" s="7" t="s">
         <v>161</v>
       </c>
-      <c r="B99" s="3" t="s">
-        <v>148</v>
-      </c>
-    </row>
-    <row r="100" spans="1:2" ht="13.8" x14ac:dyDescent="0.25">
-      <c r="A100" s="8" t="s">
+      <c r="B99" s="2" t="s">
+        <v>148</v>
+      </c>
+    </row>
+    <row r="100" spans="1:2" ht="14.25" x14ac:dyDescent="0.2">
+      <c r="A100" s="7" t="s">
         <v>162</v>
       </c>
-      <c r="B100" s="3" t="s">
-        <v>148</v>
-      </c>
-    </row>
-    <row r="101" spans="1:2" ht="13.8" x14ac:dyDescent="0.25">
-      <c r="A101" s="8" t="s">
+      <c r="B100" s="2" t="s">
+        <v>148</v>
+      </c>
+    </row>
+    <row r="101" spans="1:2" ht="14.25" x14ac:dyDescent="0.2">
+      <c r="A101" s="7" t="s">
         <v>163</v>
       </c>
-      <c r="B101" s="3" t="s">
-        <v>148</v>
-      </c>
-    </row>
-    <row r="102" spans="1:2" ht="13.8" x14ac:dyDescent="0.25">
-      <c r="A102" s="8" t="s">
+      <c r="B101" s="2" t="s">
+        <v>148</v>
+      </c>
+    </row>
+    <row r="102" spans="1:2" ht="14.25" x14ac:dyDescent="0.2">
+      <c r="A102" s="7" t="s">
         <v>164</v>
       </c>
-      <c r="B102" s="3" t="s">
-        <v>148</v>
-      </c>
-    </row>
-    <row r="103" spans="1:2" ht="13.8" x14ac:dyDescent="0.25">
-      <c r="A103" s="8" t="s">
+      <c r="B102" s="2" t="s">
+        <v>148</v>
+      </c>
+    </row>
+    <row r="103" spans="1:2" ht="14.25" x14ac:dyDescent="0.2">
+      <c r="A103" s="7" t="s">
         <v>165</v>
       </c>
-      <c r="B103" s="3" t="s">
-        <v>148</v>
-      </c>
-    </row>
-    <row r="104" spans="1:2" ht="13.8" x14ac:dyDescent="0.25">
-      <c r="A104" s="8" t="s">
+      <c r="B103" s="2" t="s">
+        <v>148</v>
+      </c>
+    </row>
+    <row r="104" spans="1:2" ht="14.25" x14ac:dyDescent="0.2">
+      <c r="A104" s="7" t="s">
         <v>166</v>
       </c>
-      <c r="B104" s="3" t="s">
-        <v>148</v>
-      </c>
-    </row>
-    <row r="105" spans="1:2" ht="13.8" x14ac:dyDescent="0.25">
-      <c r="A105" s="8" t="s">
+      <c r="B104" s="2" t="s">
+        <v>148</v>
+      </c>
+    </row>
+    <row r="105" spans="1:2" ht="14.25" x14ac:dyDescent="0.2">
+      <c r="A105" s="7" t="s">
         <v>167</v>
       </c>
-      <c r="B105" s="3" t="s">
-        <v>148</v>
-      </c>
-    </row>
-    <row r="106" spans="1:2" ht="13.8" x14ac:dyDescent="0.25">
-      <c r="A106" s="8" t="s">
+      <c r="B105" s="2" t="s">
+        <v>148</v>
+      </c>
+    </row>
+    <row r="106" spans="1:2" ht="14.25" x14ac:dyDescent="0.2">
+      <c r="A106" s="7" t="s">
         <v>168</v>
       </c>
-      <c r="B106" s="3" t="s">
-        <v>148</v>
-      </c>
-    </row>
-    <row r="107" spans="1:2" ht="13.8" x14ac:dyDescent="0.25">
-      <c r="A107" s="8" t="s">
+      <c r="B106" s="2" t="s">
+        <v>148</v>
+      </c>
+    </row>
+    <row r="107" spans="1:2" ht="14.25" x14ac:dyDescent="0.2">
+      <c r="A107" s="7" t="s">
         <v>169</v>
       </c>
-      <c r="B107" s="3" t="s">
-        <v>148</v>
-      </c>
-    </row>
-    <row r="108" spans="1:2" ht="13.8" x14ac:dyDescent="0.25">
-      <c r="A108" s="8" t="s">
+      <c r="B107" s="2" t="s">
+        <v>148</v>
+      </c>
+    </row>
+    <row r="108" spans="1:2" ht="14.25" x14ac:dyDescent="0.2">
+      <c r="A108" s="7" t="s">
         <v>170</v>
       </c>
-      <c r="B108" s="3" t="s">
-        <v>148</v>
-      </c>
-    </row>
-    <row r="109" spans="1:2" ht="13.8" x14ac:dyDescent="0.25">
-      <c r="A109" s="8" t="s">
+      <c r="B108" s="2" t="s">
+        <v>148</v>
+      </c>
+    </row>
+    <row r="109" spans="1:2" ht="14.25" x14ac:dyDescent="0.2">
+      <c r="A109" s="7" t="s">
         <v>171</v>
       </c>
-      <c r="B109" s="3" t="s">
-        <v>148</v>
-      </c>
-    </row>
-    <row r="110" spans="1:2" ht="13.8" x14ac:dyDescent="0.25">
-      <c r="A110" s="8" t="s">
+      <c r="B109" s="2" t="s">
+        <v>148</v>
+      </c>
+    </row>
+    <row r="110" spans="1:2" ht="14.25" x14ac:dyDescent="0.2">
+      <c r="A110" s="7" t="s">
         <v>172</v>
       </c>
-      <c r="B110" s="3" t="s">
-        <v>148</v>
-      </c>
-    </row>
-    <row r="111" spans="1:2" ht="13.8" x14ac:dyDescent="0.25">
-      <c r="A111" s="8" t="s">
+      <c r="B110" s="2" t="s">
+        <v>148</v>
+      </c>
+    </row>
+    <row r="111" spans="1:2" ht="14.25" x14ac:dyDescent="0.2">
+      <c r="A111" s="7" t="s">
         <v>173</v>
       </c>
-      <c r="B111" s="3" t="s">
-        <v>148</v>
-      </c>
-    </row>
-    <row r="112" spans="1:2" ht="13.8" x14ac:dyDescent="0.25">
-      <c r="A112" s="8" t="s">
+      <c r="B111" s="2" t="s">
+        <v>148</v>
+      </c>
+    </row>
+    <row r="112" spans="1:2" ht="14.25" x14ac:dyDescent="0.2">
+      <c r="A112" s="7" t="s">
         <v>174</v>
       </c>
-      <c r="B112" s="3" t="s">
-        <v>148</v>
-      </c>
-    </row>
-    <row r="113" spans="1:2" ht="13.8" x14ac:dyDescent="0.25">
-      <c r="A113" s="8" t="s">
+      <c r="B112" s="2" t="s">
+        <v>148</v>
+      </c>
+    </row>
+    <row r="113" spans="1:2" ht="14.25" x14ac:dyDescent="0.2">
+      <c r="A113" s="7" t="s">
         <v>175</v>
       </c>
-      <c r="B113" s="3" t="s">
-        <v>148</v>
-      </c>
-    </row>
-    <row r="114" spans="1:2" ht="13.8" x14ac:dyDescent="0.25">
-      <c r="A114" s="8" t="s">
+      <c r="B113" s="2" t="s">
+        <v>148</v>
+      </c>
+    </row>
+    <row r="114" spans="1:2" ht="14.25" x14ac:dyDescent="0.2">
+      <c r="A114" s="7" t="s">
         <v>176</v>
       </c>
-      <c r="B114" s="3" t="s">
-        <v>148</v>
-      </c>
-    </row>
-    <row r="115" spans="1:2" ht="13.8" x14ac:dyDescent="0.25">
-      <c r="A115" s="8" t="s">
+      <c r="B114" s="2" t="s">
+        <v>148</v>
+      </c>
+    </row>
+    <row r="115" spans="1:2" ht="14.25" x14ac:dyDescent="0.2">
+      <c r="A115" s="7" t="s">
         <v>177</v>
       </c>
-      <c r="B115" s="3" t="s">
-        <v>148</v>
-      </c>
-    </row>
-    <row r="116" spans="1:2" ht="13.8" x14ac:dyDescent="0.25">
-      <c r="A116" s="8" t="s">
+      <c r="B115" s="2" t="s">
+        <v>148</v>
+      </c>
+    </row>
+    <row r="116" spans="1:2" ht="14.25" x14ac:dyDescent="0.2">
+      <c r="A116" s="7" t="s">
         <v>178</v>
       </c>
-      <c r="B116" s="3" t="s">
-        <v>148</v>
-      </c>
-    </row>
-    <row r="117" spans="1:2" ht="13.8" x14ac:dyDescent="0.25">
-      <c r="A117" s="8" t="s">
+      <c r="B116" s="2" t="s">
+        <v>148</v>
+      </c>
+    </row>
+    <row r="117" spans="1:2" ht="14.25" x14ac:dyDescent="0.2">
+      <c r="A117" s="7" t="s">
         <v>179</v>
       </c>
-      <c r="B117" s="3" t="s">
-        <v>148</v>
-      </c>
-    </row>
-    <row r="118" spans="1:2" ht="13.8" x14ac:dyDescent="0.25">
-      <c r="A118" s="8" t="s">
+      <c r="B117" s="2" t="s">
+        <v>148</v>
+      </c>
+    </row>
+    <row r="118" spans="1:2" ht="14.25" x14ac:dyDescent="0.2">
+      <c r="A118" s="7" t="s">
         <v>180</v>
       </c>
-      <c r="B118" s="3" t="s">
-        <v>148</v>
-      </c>
-    </row>
-    <row r="119" spans="1:2" ht="13.8" x14ac:dyDescent="0.25">
-      <c r="A119" s="8" t="s">
+      <c r="B118" s="2" t="s">
+        <v>148</v>
+      </c>
+    </row>
+    <row r="119" spans="1:2" ht="14.25" x14ac:dyDescent="0.2">
+      <c r="A119" s="7" t="s">
         <v>181</v>
       </c>
-      <c r="B119" s="3" t="s">
-        <v>148</v>
-      </c>
-    </row>
-    <row r="120" spans="1:2" ht="13.8" x14ac:dyDescent="0.25">
-      <c r="A120" s="8" t="s">
+      <c r="B119" s="2" t="s">
+        <v>148</v>
+      </c>
+    </row>
+    <row r="120" spans="1:2" ht="14.25" x14ac:dyDescent="0.2">
+      <c r="A120" s="7" t="s">
         <v>76</v>
       </c>
-      <c r="B120" s="3" t="s">
+      <c r="B120" s="2" t="s">
         <v>182</v>
       </c>
     </row>
-    <row r="121" spans="1:2" ht="13.8" x14ac:dyDescent="0.25">
-      <c r="A121" s="8" t="s">
+    <row r="121" spans="1:2" ht="14.25" x14ac:dyDescent="0.2">
+      <c r="A121" s="7" t="s">
         <v>118</v>
       </c>
-      <c r="B121" s="3" t="s">
+      <c r="B121" s="2" t="s">
         <v>182</v>
       </c>
     </row>
-    <row r="1048576" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="1048576" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
   </sheetData>
   <mergeCells count="1">
     <mergeCell ref="B6:E6"/>
@@ -2490,121 +2490,123 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:E17"/>
   <sheetViews>
-    <sheetView zoomScaleNormal="100" workbookViewId="0"/>
+    <sheetView zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="A14" sqref="A14"/>
+    </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="13.2" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1025" width="14.44140625" customWidth="1"/>
+    <col min="1" max="1025" width="14.42578125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" ht="17.399999999999999" x14ac:dyDescent="0.3">
-      <c r="A1" s="2" t="s">
+    <row r="1" spans="1:5" ht="18" x14ac:dyDescent="0.25">
+      <c r="A1" s="1" t="s">
         <v>183</v>
       </c>
-      <c r="B1" s="3"/>
-    </row>
-    <row r="2" spans="1:5" ht="13.8" x14ac:dyDescent="0.25">
-      <c r="A2" s="4"/>
-      <c r="B2" s="3"/>
-    </row>
-    <row r="3" spans="1:5" ht="13.8" x14ac:dyDescent="0.25">
-      <c r="A3" s="4" t="s">
+      <c r="B1" s="2"/>
+    </row>
+    <row r="2" spans="1:5" ht="15" x14ac:dyDescent="0.25">
+      <c r="A2" s="3"/>
+      <c r="B2" s="2"/>
+    </row>
+    <row r="3" spans="1:5" ht="15" x14ac:dyDescent="0.25">
+      <c r="A3" s="3" t="s">
         <v>1</v>
       </c>
-      <c r="B3" s="5" t="s">
+      <c r="B3" s="4" t="s">
         <v>184</v>
       </c>
     </row>
-    <row r="4" spans="1:5" ht="13.8" x14ac:dyDescent="0.25">
-      <c r="A4" s="4" t="s">
+    <row r="4" spans="1:5" ht="15" x14ac:dyDescent="0.25">
+      <c r="A4" s="3" t="s">
         <v>3</v>
       </c>
-      <c r="B4" s="5">
+      <c r="B4" s="4">
         <v>1</v>
       </c>
     </row>
-    <row r="5" spans="1:5" ht="13.8" x14ac:dyDescent="0.25">
-      <c r="A5" s="4" t="s">
+    <row r="5" spans="1:5" ht="15" x14ac:dyDescent="0.25">
+      <c r="A5" s="3" t="s">
         <v>4</v>
       </c>
-      <c r="B5" s="5">
+      <c r="B5" s="4">
         <v>2015</v>
       </c>
     </row>
-    <row r="6" spans="1:5" ht="13.8" x14ac:dyDescent="0.25">
-      <c r="A6" s="4" t="s">
+    <row r="6" spans="1:5" ht="15" x14ac:dyDescent="0.25">
+      <c r="A6" s="3" t="s">
         <v>5</v>
       </c>
-      <c r="B6" s="1"/>
-      <c r="C6" s="1"/>
-      <c r="D6" s="1"/>
-      <c r="E6" s="1"/>
-    </row>
-    <row r="7" spans="1:5" ht="13.8" x14ac:dyDescent="0.25">
-      <c r="A7" s="3"/>
-      <c r="B7" s="3"/>
-      <c r="C7" s="3"/>
-      <c r="D7" s="3"/>
-      <c r="E7" s="3"/>
-    </row>
-    <row r="8" spans="1:5" ht="13.8" x14ac:dyDescent="0.25">
-      <c r="A8" s="7" t="s">
+      <c r="B6" s="15"/>
+      <c r="C6" s="15"/>
+      <c r="D6" s="15"/>
+      <c r="E6" s="15"/>
+    </row>
+    <row r="7" spans="1:5" ht="14.25" x14ac:dyDescent="0.2">
+      <c r="A7" s="2"/>
+      <c r="B7" s="2"/>
+      <c r="C7" s="2"/>
+      <c r="D7" s="2"/>
+      <c r="E7" s="2"/>
+    </row>
+    <row r="8" spans="1:5" ht="15" x14ac:dyDescent="0.2">
+      <c r="A8" s="6" t="s">
         <v>6</v>
       </c>
-      <c r="B8" s="7" t="s">
+      <c r="B8" s="6" t="s">
         <v>7</v>
       </c>
-      <c r="C8" s="7" t="s">
+      <c r="C8" s="6" t="s">
         <v>8</v>
       </c>
-      <c r="D8" s="7" t="s">
+      <c r="D8" s="6" t="s">
         <v>5</v>
       </c>
-      <c r="E8" s="7" t="s">
+      <c r="E8" s="6" t="s">
         <v>9</v>
       </c>
     </row>
-    <row r="9" spans="1:5" ht="13.8" x14ac:dyDescent="0.25">
-      <c r="A9" s="3" t="s">
+    <row r="9" spans="1:5" ht="14.25" x14ac:dyDescent="0.2">
+      <c r="A9" s="2" t="s">
         <v>185</v>
       </c>
     </row>
-    <row r="10" spans="1:5" ht="13.8" x14ac:dyDescent="0.25">
-      <c r="A10" s="3" t="s">
+    <row r="10" spans="1:5" ht="14.25" x14ac:dyDescent="0.2">
+      <c r="A10" s="2" t="s">
         <v>10</v>
       </c>
     </row>
-    <row r="11" spans="1:5" ht="13.8" x14ac:dyDescent="0.25">
-      <c r="A11" s="3" t="s">
+    <row r="11" spans="1:5" ht="14.25" x14ac:dyDescent="0.2">
+      <c r="A11" s="2" t="s">
         <v>37</v>
       </c>
     </row>
-    <row r="12" spans="1:5" ht="13.8" x14ac:dyDescent="0.25">
-      <c r="A12" s="3" t="s">
+    <row r="12" spans="1:5" ht="14.25" x14ac:dyDescent="0.2">
+      <c r="A12" s="2" t="s">
         <v>186</v>
       </c>
     </row>
-    <row r="13" spans="1:5" ht="13.8" x14ac:dyDescent="0.25">
-      <c r="A13" s="3" t="s">
+    <row r="13" spans="1:5" ht="14.25" x14ac:dyDescent="0.2">
+      <c r="A13" s="2" t="s">
         <v>187</v>
       </c>
     </row>
-    <row r="14" spans="1:5" ht="13.8" x14ac:dyDescent="0.25">
-      <c r="A14" s="3" t="s">
+    <row r="14" spans="1:5" ht="14.25" x14ac:dyDescent="0.2">
+      <c r="A14" s="2" t="s">
         <v>188</v>
       </c>
     </row>
-    <row r="16" spans="1:5" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A16" s="11" t="s">
+    <row r="16" spans="1:5" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A16" s="10" t="s">
         <v>145</v>
       </c>
-      <c r="B16" s="13"/>
-    </row>
-    <row r="17" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A17" s="14" t="s">
+      <c r="B16" s="12"/>
+    </row>
+    <row r="17" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A17" s="13" t="s">
         <v>6</v>
       </c>
-      <c r="B17" s="14" t="s">
+      <c r="B17" s="13" t="s">
         <v>146</v>
       </c>
     </row>

</xml_diff>